<commit_message>
made changes to codebook
</commit_message>
<xml_diff>
--- a/data/Codebook-Ranatunga-Ashvin.xlsx
+++ b/data/Codebook-Ranatunga-Ashvin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashvi\Documents\Monash\ETC5512\Assignments\Assignment_4\A4_5512\assignment4_30301343\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashvi\Documents\Monash\ETC5512\Assignments\Assignment_4\A4_5512\assignment4_30301343\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2073A163-B135-497F-A80C-B7AC5F6EEB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBF4D00-E425-450D-8FFB-F2C2EE532870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{82B17F62-FDC3-4B52-86C3-0878166F623D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>diagnosis_date</t>
   </si>
@@ -50,9 +50,6 @@
     <t>This referes to the total number of cases diagnosed on a given date</t>
   </si>
   <si>
-    <t>This variable differentiates between the cases that occur on the 2 intervention dates required and the other dates</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>Numeric</t>
   </si>
   <si>
-    <t>Alphabet</t>
-  </si>
-  <si>
     <t>Format</t>
   </si>
   <si>
@@ -101,16 +95,7 @@
     <t>Total Number of Cases</t>
   </si>
   <si>
-    <t>Type of Date</t>
-  </si>
-  <si>
     <t>This was derived by adding all the cases according to each respective date</t>
-  </si>
-  <si>
-    <t>type_of_date</t>
-  </si>
-  <si>
-    <t>This variable was derived to quantify the effects local lockdowns and face coverings on the dates of intervention that were requested. It contains the following:                                             date_of_intervention= The 2 requested dates                                                           other = All other dates</t>
   </si>
 </sst>
 </file>
@@ -514,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C7D8DFA-6D7D-49AF-A7A6-12B4245D1182}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -533,7 +518,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -541,25 +526,25 @@
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.35">
@@ -570,22 +555,22 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.35">
@@ -596,48 +581,22 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" ht="127" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>